<commit_message>
update testcase by spin
</commit_message>
<xml_diff>
--- a/Document/Test-case-EWSD.xlsx
+++ b/Document/Test-case-EWSD.xlsx
@@ -5,14 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EWSD\COMP1640_CW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EWSD\COMP1640_CW\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
   </bookViews>
   <sheets>
-    <sheet name="Test case EWSD" sheetId="1" r:id="rId1"/>
+    <sheet name="Test case - all" sheetId="1" r:id="rId1"/>
+    <sheet name="Spin 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Spin 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Spin 3" sheetId="4" r:id="rId4"/>
+    <sheet name="Spin 4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="213">
   <si>
     <t>Test numb</t>
   </si>
@@ -758,7 +762,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -859,35 +863,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -923,29 +905,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -965,18 +929,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -987,6 +960,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1272,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,10 +1287,10 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="2" t="s">
         <v>98</v>
       </c>
@@ -1320,10 +1314,10 @@
       <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1328,7 @@
         <v>17</v>
       </c>
       <c r="G4" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>24</v>
@@ -1347,8 +1341,8 @@
       <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1353,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>24</v>
@@ -1372,8 +1366,8 @@
       <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1384,7 +1378,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>16</v>
@@ -1397,8 +1391,8 @@
       <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1409,7 +1403,7 @@
         <v>21</v>
       </c>
       <c r="G7" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H7" s="11" t="s">
         <v>24</v>
@@ -1422,8 +1416,8 @@
       <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1428,7 @@
         <v>21</v>
       </c>
       <c r="G8" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>24</v>
@@ -1447,8 +1441,8 @@
       <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1459,7 +1453,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>23</v>
@@ -1472,10 +1466,10 @@
       <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="27"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="3" t="s">
         <v>176</v>
       </c>
@@ -1486,7 +1480,7 @@
         <v>178</v>
       </c>
       <c r="G10" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>179</v>
@@ -1499,10 +1493,10 @@
       <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="35" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1515,7 +1509,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>34</v>
@@ -1528,7 +1522,7 @@
       <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
@@ -1542,7 +1536,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>35</v>
@@ -1555,8 +1549,8 @@
       <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1569,7 +1563,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>24</v>
@@ -1582,8 +1576,8 @@
       <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="15"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1594,7 +1588,7 @@
         <v>39</v>
       </c>
       <c r="G14" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>24</v>
@@ -1607,8 +1601,8 @@
       <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="6" t="s">
         <v>41</v>
       </c>
@@ -1619,7 +1613,7 @@
         <v>43</v>
       </c>
       <c r="G15" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>40</v>
@@ -1632,8 +1626,8 @@
       <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="6" t="s">
         <v>75</v>
       </c>
@@ -1644,7 +1638,7 @@
         <v>44</v>
       </c>
       <c r="G16" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>45</v>
@@ -1657,8 +1651,8 @@
       <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1671,7 +1665,7 @@
         <v>38</v>
       </c>
       <c r="G17" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>24</v>
@@ -1684,8 +1678,8 @@
       <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="3" t="s">
         <v>37</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>39</v>
       </c>
       <c r="G18" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H18" s="11" t="s">
         <v>24</v>
@@ -1709,8 +1703,8 @@
       <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="6" t="s">
         <v>47</v>
       </c>
@@ -1721,7 +1715,7 @@
         <v>48</v>
       </c>
       <c r="G19" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>40</v>
@@ -1734,8 +1728,8 @@
       <c r="A20" s="5">
         <v>17</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="6" t="s">
         <v>73</v>
       </c>
@@ -1746,7 +1740,7 @@
         <v>49</v>
       </c>
       <c r="G20" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>45</v>
@@ -1759,8 +1753,8 @@
       <c r="A21" s="5">
         <v>18</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="12" t="s">
+      <c r="B21" s="28"/>
+      <c r="C21" s="24" t="s">
         <v>50</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -1773,7 +1767,7 @@
         <v>52</v>
       </c>
       <c r="G21" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>40</v>
@@ -1786,8 +1780,8 @@
       <c r="A22" s="5">
         <v>19</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="6" t="s">
         <v>53</v>
       </c>
@@ -1798,7 +1792,7 @@
         <v>54</v>
       </c>
       <c r="G22" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>55</v>
@@ -1811,8 +1805,8 @@
       <c r="A23" s="5">
         <v>20</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="6" t="s">
         <v>56</v>
       </c>
@@ -1823,7 +1817,7 @@
         <v>57</v>
       </c>
       <c r="G23" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>58</v>
@@ -1836,7 +1830,7 @@
       <c r="A24" s="5">
         <v>21</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="24" t="s">
         <v>60</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -1852,7 +1846,7 @@
         <v>34</v>
       </c>
       <c r="G24" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>34</v>
@@ -1865,7 +1859,7 @@
       <c r="A25" s="5">
         <v>22</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="10" t="s">
         <v>61</v>
       </c>
@@ -1879,7 +1873,7 @@
         <v>35</v>
       </c>
       <c r="G25" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>35</v>
@@ -1892,8 +1886,8 @@
       <c r="A26" s="5">
         <v>23</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24" t="s">
         <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -1906,7 +1900,7 @@
         <v>67</v>
       </c>
       <c r="G26" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>24</v>
@@ -1919,8 +1913,8 @@
       <c r="A27" s="5">
         <v>24</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="3" t="s">
         <v>66</v>
       </c>
@@ -1931,7 +1925,7 @@
         <v>68</v>
       </c>
       <c r="G27" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H27" s="11" t="s">
         <v>24</v>
@@ -1944,8 +1938,8 @@
       <c r="A28" s="5">
         <v>25</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="3" t="s">
         <v>9</v>
       </c>
@@ -1956,7 +1950,7 @@
         <v>69</v>
       </c>
       <c r="G28" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H28" s="11" t="s">
         <v>24</v>
@@ -1969,8 +1963,8 @@
       <c r="A29" s="5">
         <v>26</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="3" t="s">
         <v>70</v>
       </c>
@@ -1981,7 +1975,7 @@
         <v>71</v>
       </c>
       <c r="G29" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H29" s="11" t="s">
         <v>24</v>
@@ -1994,8 +1988,8 @@
       <c r="A30" s="5">
         <v>27</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="6" t="s">
         <v>74</v>
       </c>
@@ -2006,7 +2000,7 @@
         <v>76</v>
       </c>
       <c r="G30" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>45</v>
@@ -2019,8 +2013,8 @@
       <c r="A31" s="5">
         <v>28</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2033,7 +2027,7 @@
         <v>67</v>
       </c>
       <c r="G31" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>24</v>
@@ -2046,8 +2040,8 @@
       <c r="A32" s="5">
         <v>29</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="3" t="s">
         <v>66</v>
       </c>
@@ -2058,7 +2052,7 @@
         <v>68</v>
       </c>
       <c r="G32" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H32" s="11" t="s">
         <v>24</v>
@@ -2071,8 +2065,8 @@
       <c r="A33" s="5">
         <v>30</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="3" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2077,7 @@
         <v>69</v>
       </c>
       <c r="G33" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>24</v>
@@ -2096,8 +2090,8 @@
       <c r="A34" s="5">
         <v>31</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="3" t="s">
         <v>70</v>
       </c>
@@ -2108,7 +2102,7 @@
         <v>71</v>
       </c>
       <c r="G34" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H34" s="11" t="s">
         <v>24</v>
@@ -2121,8 +2115,8 @@
       <c r="A35" s="5">
         <v>32</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="6" t="s">
         <v>73</v>
       </c>
@@ -2133,7 +2127,7 @@
         <v>79</v>
       </c>
       <c r="G35" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>45</v>
@@ -2146,7 +2140,7 @@
       <c r="A36" s="5">
         <v>33</v>
       </c>
-      <c r="B36" s="12"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="1" t="s">
         <v>80</v>
       </c>
@@ -2160,7 +2154,7 @@
         <v>82</v>
       </c>
       <c r="G36" s="8">
-        <v>42445</v>
+        <v>42473</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>83</v>
@@ -2173,28 +2167,28 @@
       <c r="A37" s="5">
         <v>34</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="21" t="s">
+      <c r="D37" s="15" t="s">
         <v>118</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="16">
-        <v>42473</v>
-      </c>
-      <c r="H37" s="22" t="s">
+      <c r="G37" s="8">
+        <v>42473</v>
+      </c>
+      <c r="H37" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I37" s="17" t="s">
+      <c r="I37" s="14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2202,11 +2196,11 @@
       <c r="A38" s="5">
         <v>35</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="15" t="s">
         <v>121</v>
       </c>
       <c r="E38" s="6" t="s">
@@ -2215,7 +2209,7 @@
       <c r="F38" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G38" s="16">
+      <c r="G38" s="8">
         <v>42473</v>
       </c>
       <c r="H38" s="6" t="s">
@@ -2229,20 +2223,20 @@
       <c r="A39" s="5">
         <v>36</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="18" t="s">
+      <c r="B39" s="24"/>
+      <c r="C39" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="23">
+      <c r="E39" s="17">
         <v>1</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="8">
         <v>42473</v>
       </c>
       <c r="H39" s="11" t="s">
@@ -2256,8 +2250,8 @@
       <c r="A40" s="5">
         <v>37</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="19"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="28"/>
       <c r="D40" s="6" t="s">
         <v>99</v>
       </c>
@@ -2267,7 +2261,7 @@
       <c r="F40" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="8">
         <v>42473</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -2281,8 +2275,8 @@
       <c r="A41" s="5">
         <v>38</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="19"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="28"/>
       <c r="D41" s="6" t="s">
         <v>100</v>
       </c>
@@ -2292,7 +2286,7 @@
       <c r="F41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="16">
+      <c r="G41" s="8">
         <v>42473</v>
       </c>
       <c r="H41" s="11" t="s">
@@ -2306,8 +2300,8 @@
       <c r="A42" s="5">
         <v>39</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="28"/>
       <c r="D42" s="6" t="s">
         <v>101</v>
       </c>
@@ -2317,7 +2311,7 @@
       <c r="F42" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="16">
+      <c r="G42" s="8">
         <v>42473</v>
       </c>
       <c r="H42" s="11" t="s">
@@ -2331,8 +2325,8 @@
       <c r="A43" s="5">
         <v>40</v>
       </c>
-      <c r="B43" s="12"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="28"/>
       <c r="D43" s="6" t="s">
         <v>102</v>
       </c>
@@ -2342,7 +2336,7 @@
       <c r="F43" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="8">
         <v>42473</v>
       </c>
       <c r="H43" s="11" t="s">
@@ -2356,24 +2350,24 @@
       <c r="A44" s="5">
         <v>41</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="23" t="s">
+      <c r="B44" s="24"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E44" s="25" t="s">
+      <c r="E44" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F44" s="23" t="s">
+      <c r="F44" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="16">
-        <v>42473</v>
-      </c>
-      <c r="H44" s="26" t="s">
+      <c r="G44" s="8">
+        <v>42473</v>
+      </c>
+      <c r="H44" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="I44" s="26" t="s">
+      <c r="I44" s="20" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2381,8 +2375,8 @@
       <c r="A45" s="5">
         <v>42</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="18" t="s">
+      <c r="B45" s="24"/>
+      <c r="C45" s="27" t="s">
         <v>90</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2394,7 +2388,7 @@
       <c r="F45" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="8">
         <v>42473</v>
       </c>
       <c r="H45" s="11" t="s">
@@ -2408,8 +2402,8 @@
       <c r="A46" s="5">
         <v>43</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="19"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="6" t="s">
         <v>101</v>
       </c>
@@ -2419,7 +2413,7 @@
       <c r="F46" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G46" s="16">
+      <c r="G46" s="8">
         <v>42473</v>
       </c>
       <c r="H46" s="11" t="s">
@@ -2433,8 +2427,8 @@
       <c r="A47" s="5">
         <v>44</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="19"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="28"/>
       <c r="D47" s="6" t="s">
         <v>102</v>
       </c>
@@ -2444,7 +2438,7 @@
       <c r="F47" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="16">
+      <c r="G47" s="8">
         <v>42473</v>
       </c>
       <c r="H47" s="11" t="s">
@@ -2458,24 +2452,24 @@
       <c r="A48" s="5">
         <v>45</v>
       </c>
-      <c r="B48" s="12"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="23" t="s">
+      <c r="B48" s="24"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F48" s="23" t="s">
+      <c r="F48" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G48" s="16">
-        <v>42473</v>
-      </c>
-      <c r="H48" s="26" t="s">
+      <c r="G48" s="8">
+        <v>42473</v>
+      </c>
+      <c r="H48" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="I48" s="20" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2483,7 +2477,7 @@
       <c r="A49" s="5">
         <v>46</v>
       </c>
-      <c r="B49" s="12"/>
+      <c r="B49" s="24"/>
       <c r="C49" s="1" t="s">
         <v>91</v>
       </c>
@@ -2510,10 +2504,10 @@
       <c r="A50" s="5">
         <v>47</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="23" t="s">
         <v>117</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -2539,11 +2533,11 @@
       <c r="A51" s="5">
         <v>48</v>
       </c>
-      <c r="B51" s="19"/>
-      <c r="C51" s="30" t="s">
+      <c r="B51" s="28"/>
+      <c r="C51" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="D51" s="15" t="s">
         <v>122</v>
       </c>
       <c r="E51" s="6" t="s">
@@ -2566,8 +2560,8 @@
       <c r="A52" s="5">
         <v>49</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="31" t="s">
+      <c r="B52" s="28"/>
+      <c r="C52" s="25" t="s">
         <v>125</v>
       </c>
       <c r="D52" s="6" t="s">
@@ -2593,8 +2587,8 @@
       <c r="A53" s="5">
         <v>50</v>
       </c>
-      <c r="B53" s="19"/>
-      <c r="C53" s="31"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="25"/>
       <c r="D53" s="3" t="s">
         <v>127</v>
       </c>
@@ -2618,8 +2612,8 @@
       <c r="A54" s="5">
         <v>51</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="31"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="25"/>
       <c r="D54" s="3" t="s">
         <v>128</v>
       </c>
@@ -2643,8 +2637,8 @@
       <c r="A55" s="5">
         <v>52</v>
       </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="31"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="25"/>
       <c r="D55" s="3" t="s">
         <v>66</v>
       </c>
@@ -2668,8 +2662,8 @@
       <c r="A56" s="5">
         <v>53</v>
       </c>
-      <c r="B56" s="19"/>
-      <c r="C56" s="31"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="25"/>
       <c r="D56" s="3" t="s">
         <v>129</v>
       </c>
@@ -2693,8 +2687,8 @@
       <c r="A57" s="5">
         <v>54</v>
       </c>
-      <c r="B57" s="19"/>
-      <c r="C57" s="31"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="25"/>
       <c r="D57" s="6" t="s">
         <v>73</v>
       </c>
@@ -2707,7 +2701,7 @@
       <c r="G57" s="8">
         <v>42473</v>
       </c>
-      <c r="H57" s="29" t="s">
+      <c r="H57" s="22" t="s">
         <v>137</v>
       </c>
       <c r="I57" s="6" t="s">
@@ -2718,8 +2712,8 @@
       <c r="A58" s="5">
         <v>55</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="33" t="s">
+      <c r="B58" s="28"/>
+      <c r="C58" s="30" t="s">
         <v>173</v>
       </c>
       <c r="D58" s="6" t="s">
@@ -2745,8 +2739,8 @@
       <c r="A59" s="5">
         <v>56</v>
       </c>
-      <c r="B59" s="19"/>
-      <c r="C59" s="34"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="31"/>
       <c r="D59" s="3" t="s">
         <v>127</v>
       </c>
@@ -2770,8 +2764,8 @@
       <c r="A60" s="5">
         <v>57</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="34"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="3" t="s">
         <v>128</v>
       </c>
@@ -2795,8 +2789,8 @@
       <c r="A61" s="5">
         <v>58</v>
       </c>
-      <c r="B61" s="19"/>
-      <c r="C61" s="34"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="31"/>
       <c r="D61" s="3" t="s">
         <v>66</v>
       </c>
@@ -2820,8 +2814,8 @@
       <c r="A62" s="5">
         <v>59</v>
       </c>
-      <c r="B62" s="19"/>
-      <c r="C62" s="34"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="3" t="s">
         <v>129</v>
       </c>
@@ -2845,8 +2839,8 @@
       <c r="A63" s="5">
         <v>60</v>
       </c>
-      <c r="B63" s="19"/>
-      <c r="C63" s="35"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="32"/>
       <c r="D63" s="6" t="s">
         <v>73</v>
       </c>
@@ -2856,8 +2850,10 @@
       <c r="F63" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G63" s="8"/>
-      <c r="H63" s="26" t="s">
+      <c r="G63" s="8">
+        <v>42473</v>
+      </c>
+      <c r="H63" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I63" s="6" t="s">
@@ -2868,8 +2864,8 @@
       <c r="A64" s="5">
         <v>61</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="28" t="s">
+      <c r="B64" s="29"/>
+      <c r="C64" s="21" t="s">
         <v>138</v>
       </c>
       <c r="D64" s="6" t="s">
@@ -2895,10 +2891,10 @@
       <c r="A65" s="5">
         <v>62</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="28" t="s">
+      <c r="C65" s="21" t="s">
         <v>141</v>
       </c>
       <c r="D65" s="6" t="s">
@@ -2924,8 +2920,8 @@
       <c r="A66" s="5">
         <v>63</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="28" t="s">
+      <c r="B66" s="24"/>
+      <c r="C66" s="21" t="s">
         <v>142</v>
       </c>
       <c r="D66" s="6" t="s">
@@ -2951,8 +2947,8 @@
       <c r="A67" s="5">
         <v>64</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="15" t="s">
+      <c r="B67" s="24"/>
+      <c r="C67" s="26" t="s">
         <v>147</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -2978,8 +2974,8 @@
       <c r="A68" s="5">
         <v>65</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="15"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="26"/>
       <c r="D68" s="1" t="s">
         <v>151</v>
       </c>
@@ -3003,8 +2999,8 @@
       <c r="A69" s="5">
         <v>66</v>
       </c>
-      <c r="B69" s="12"/>
-      <c r="C69" s="15"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="1" t="s">
         <v>152</v>
       </c>
@@ -3028,8 +3024,8 @@
       <c r="A70" s="5">
         <v>67</v>
       </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="15"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="26"/>
       <c r="D70" s="1" t="s">
         <v>153</v>
       </c>
@@ -3053,8 +3049,8 @@
       <c r="A71" s="5">
         <v>68</v>
       </c>
-      <c r="B71" s="12"/>
-      <c r="C71" s="15"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="26"/>
       <c r="D71" s="1" t="s">
         <v>154</v>
       </c>
@@ -3078,8 +3074,8 @@
       <c r="A72" s="5">
         <v>69</v>
       </c>
-      <c r="B72" s="12"/>
-      <c r="C72" s="15"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="26"/>
       <c r="D72" s="1" t="s">
         <v>155</v>
       </c>
@@ -3103,12 +3099,12 @@
       <c r="A73" s="5">
         <v>70</v>
       </c>
-      <c r="B73" s="12"/>
-      <c r="C73" s="15"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="26"/>
       <c r="D73" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E73" s="24" t="s">
+      <c r="E73" s="18" t="s">
         <v>157</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -3128,12 +3124,12 @@
       <c r="A74" s="5">
         <v>71</v>
       </c>
-      <c r="B74" s="12"/>
-      <c r="C74" s="15"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="26"/>
       <c r="D74" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E74" s="24" t="s">
+      <c r="E74" s="18" t="s">
         <v>156</v>
       </c>
       <c r="F74" s="3" t="s">
@@ -3153,12 +3149,12 @@
       <c r="A75" s="5">
         <v>72</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="15"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="26"/>
       <c r="D75" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E75" s="24" t="s">
+      <c r="E75" s="18" t="s">
         <v>172</v>
       </c>
       <c r="F75" s="6" t="s">
@@ -3178,8 +3174,8 @@
       <c r="A76" s="5">
         <v>73</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="18" t="s">
+      <c r="B76" s="24"/>
+      <c r="C76" s="27" t="s">
         <v>168</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -3205,8 +3201,8 @@
       <c r="A77" s="5">
         <v>74</v>
       </c>
-      <c r="B77" s="12"/>
-      <c r="C77" s="19"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="28"/>
       <c r="D77" s="1" t="s">
         <v>151</v>
       </c>
@@ -3230,8 +3226,8 @@
       <c r="A78" s="5">
         <v>75</v>
       </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="19"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="28"/>
       <c r="D78" s="1" t="s">
         <v>152</v>
       </c>
@@ -3255,8 +3251,8 @@
       <c r="A79" s="5">
         <v>76</v>
       </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="19"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="28"/>
       <c r="D79" s="1" t="s">
         <v>153</v>
       </c>
@@ -3280,8 +3276,8 @@
       <c r="A80" s="5">
         <v>77</v>
       </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="19"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="28"/>
       <c r="D80" s="1" t="s">
         <v>154</v>
       </c>
@@ -3305,8 +3301,8 @@
       <c r="A81" s="5">
         <v>78</v>
       </c>
-      <c r="B81" s="12"/>
-      <c r="C81" s="19"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="28"/>
       <c r="D81" s="1" t="s">
         <v>155</v>
       </c>
@@ -3330,12 +3326,12 @@
       <c r="A82" s="5">
         <v>79</v>
       </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="19"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="28"/>
       <c r="D82" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E82" s="24" t="s">
+      <c r="E82" s="18" t="s">
         <v>157</v>
       </c>
       <c r="F82" s="3" t="s">
@@ -3355,12 +3351,12 @@
       <c r="A83" s="5">
         <v>80</v>
       </c>
-      <c r="B83" s="12"/>
-      <c r="C83" s="19"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="28"/>
       <c r="D83" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E83" s="24" t="s">
+      <c r="E83" s="18" t="s">
         <v>156</v>
       </c>
       <c r="F83" s="3" t="s">
@@ -3380,8 +3376,8 @@
       <c r="A84" s="5">
         <v>81</v>
       </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="20"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="29"/>
       <c r="D84" s="1" t="s">
         <v>73</v>
       </c>
@@ -3405,11 +3401,11 @@
       <c r="A85" s="5">
         <v>82</v>
       </c>
-      <c r="B85" s="12"/>
-      <c r="C85" s="28" t="s">
+      <c r="B85" s="24"/>
+      <c r="C85" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="D85" s="28" t="s">
+      <c r="D85" s="21" t="s">
         <v>95</v>
       </c>
       <c r="E85" s="1" t="s">
@@ -3432,11 +3428,11 @@
       <c r="A86" s="5">
         <v>83</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="28" t="s">
+      <c r="C86" s="24"/>
+      <c r="D86" s="21" t="s">
         <v>184</v>
       </c>
       <c r="E86" s="6" t="s">
@@ -3459,9 +3455,9 @@
       <c r="A87" s="5">
         <v>84</v>
       </c>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="28" t="s">
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="21" t="s">
         <v>185</v>
       </c>
       <c r="E87" s="6" t="s">
@@ -3484,9 +3480,9 @@
       <c r="A88" s="5">
         <v>85</v>
       </c>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="28" t="s">
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="21" t="s">
         <v>186</v>
       </c>
       <c r="E88" s="6" t="s">
@@ -3509,11 +3505,11 @@
       <c r="A89" s="5">
         <v>86</v>
       </c>
-      <c r="B89" s="12" t="s">
+      <c r="B89" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C89" s="12"/>
-      <c r="D89" s="28" t="s">
+      <c r="C89" s="24"/>
+      <c r="D89" s="21" t="s">
         <v>194</v>
       </c>
       <c r="E89" s="6" t="s">
@@ -3536,15 +3532,15 @@
       <c r="A90" s="5">
         <v>87</v>
       </c>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="28" t="s">
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="21" t="s">
         <v>185</v>
       </c>
       <c r="E90" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F90" s="17" t="s">
+      <c r="F90" s="14" t="s">
         <v>190</v>
       </c>
       <c r="G90" s="8">
@@ -3561,9 +3557,9 @@
       <c r="A91" s="5">
         <v>88</v>
       </c>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="28" t="s">
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="21" t="s">
         <v>195</v>
       </c>
       <c r="E91" s="6" t="s">
@@ -3575,7 +3571,7 @@
       <c r="G91" s="8">
         <v>42473</v>
       </c>
-      <c r="H91" s="28" t="s">
+      <c r="H91" s="21" t="s">
         <v>197</v>
       </c>
       <c r="I91" s="6" t="s">
@@ -3586,11 +3582,11 @@
       <c r="A92" s="5">
         <v>89</v>
       </c>
-      <c r="B92" s="12" t="s">
+      <c r="B92" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C92" s="12"/>
-      <c r="D92" s="28" t="s">
+      <c r="C92" s="24"/>
+      <c r="D92" s="21" t="s">
         <v>199</v>
       </c>
       <c r="E92" s="6" t="s">
@@ -3613,15 +3609,15 @@
       <c r="A93" s="5">
         <v>90</v>
       </c>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="28" t="s">
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="21" t="s">
         <v>200</v>
       </c>
       <c r="E93" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F93" s="17" t="s">
+      <c r="F93" s="14" t="s">
         <v>190</v>
       </c>
       <c r="G93" s="8">
@@ -3638,9 +3634,9 @@
       <c r="A94" s="5">
         <v>91</v>
       </c>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="28" t="s">
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="21" t="s">
         <v>201</v>
       </c>
       <c r="E94" s="6" t="s">
@@ -3652,7 +3648,7 @@
       <c r="G94" s="8">
         <v>42473</v>
       </c>
-      <c r="H94" s="28" t="s">
+      <c r="H94" s="21" t="s">
         <v>197</v>
       </c>
       <c r="I94" s="6" t="s">
@@ -3663,11 +3659,11 @@
       <c r="A95" s="5">
         <v>92</v>
       </c>
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="C95" s="12"/>
-      <c r="D95" s="28" t="s">
+      <c r="C95" s="24"/>
+      <c r="D95" s="21" t="s">
         <v>204</v>
       </c>
       <c r="E95" s="6" t="s">
@@ -3690,9 +3686,9 @@
       <c r="A96" s="5">
         <v>93</v>
       </c>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="28" t="s">
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="21" t="s">
         <v>205</v>
       </c>
       <c r="E96" s="6" t="s">
@@ -3715,9 +3711,9 @@
       <c r="A97" s="5">
         <v>94</v>
       </c>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="28" t="s">
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="21" t="s">
         <v>206</v>
       </c>
       <c r="E97" s="6" t="s">
@@ -3729,7 +3725,7 @@
       <c r="G97" s="8">
         <v>42473</v>
       </c>
-      <c r="H97" s="28" t="s">
+      <c r="H97" s="21" t="s">
         <v>209</v>
       </c>
       <c r="I97" s="6" t="s">
@@ -3740,9 +3736,9 @@
       <c r="A98" s="5">
         <v>95</v>
       </c>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="28" t="s">
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="21" t="s">
         <v>210</v>
       </c>
       <c r="E98" s="6" t="s">
@@ -3754,7 +3750,7 @@
       <c r="G98" s="8">
         <v>42473</v>
       </c>
-      <c r="H98" s="28" t="s">
+      <c r="H98" s="21" t="s">
         <v>212</v>
       </c>
       <c r="I98" s="6" t="s">
@@ -3763,16 +3759,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B86:C88"/>
-    <mergeCell ref="B89:C91"/>
-    <mergeCell ref="B92:C94"/>
-    <mergeCell ref="B95:C98"/>
-    <mergeCell ref="C52:C57"/>
-    <mergeCell ref="C67:C75"/>
-    <mergeCell ref="C76:C84"/>
-    <mergeCell ref="B50:B64"/>
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="B65:B85"/>
     <mergeCell ref="B4:C9"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="C13:C16"/>
@@ -3786,8 +3772,2711 @@
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="C26:C30"/>
+    <mergeCell ref="B86:C88"/>
+    <mergeCell ref="B89:C91"/>
+    <mergeCell ref="B92:C94"/>
+    <mergeCell ref="B95:C98"/>
+    <mergeCell ref="C52:C57"/>
+    <mergeCell ref="C67:C75"/>
+    <mergeCell ref="C76:C84"/>
+    <mergeCell ref="B50:B64"/>
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="B65:B85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>25</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>26</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="8">
+        <v>42405</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:B14"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B27"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C22:C26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="8">
+        <v>42415</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G20" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G21" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G24" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>24</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>25</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>26</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
+        <v>27</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
+        <v>28</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G29" s="8">
+        <v>42420</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:B29"/>
+    <mergeCell ref="C11:C19"/>
+    <mergeCell ref="C20:C28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G4" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G6" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G7" s="8">
+        <v>42432</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G17" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" s="13">
+        <v>42439</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="B8:B20"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="C16:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G3" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G6" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="G7" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>14</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G15" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>16</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>17</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>18</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="28"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G20" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G22" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>22</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G23" s="8">
+        <v>42444</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="B5:C8"/>
+    <mergeCell ref="B9:B23"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="C17:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>